<commit_message>
Completed prediction stats and visualization.
</commit_message>
<xml_diff>
--- a/SoCalEdison Bills.xlsx
+++ b/SoCalEdison Bills.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UserLo\source\repos\learning\SoCalEdison\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UserLo\source\repos\learning\SCEdison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AD0317-2FAA-455C-8372-57062E3BF04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ED894E-8A75-47BB-ACBF-90F0FC66EF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="240" windowWidth="23745" windowHeight="12285" activeTab="1" xr2:uid="{52A8A652-56DC-477E-BCA1-00D231B19864}"/>
+    <workbookView xWindow="3045" yWindow="240" windowWidth="23745" windowHeight="12285" activeTab="2" xr2:uid="{52A8A652-56DC-477E-BCA1-00D231B19864}"/>
   </bookViews>
   <sheets>
     <sheet name="Bills" sheetId="8" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Projections" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="36">
   <si>
     <t>Bill</t>
   </si>
@@ -44,9 +43,6 @@
     <t>Jun</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>May</t>
   </si>
   <si>
@@ -86,9 +82,6 @@
     <t>year</t>
   </si>
   <si>
-    <t>Amt</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -147,6 +140,9 @@
   </si>
   <si>
     <t>climate_credit</t>
+  </si>
+  <si>
+    <t>amt</t>
   </si>
 </sst>
 </file>
@@ -155,7 +151,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="169" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -191,7 +187,7 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB72E51-01F8-41C6-BBC4-A5EAE2717D03}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,66 +513,66 @@
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="4" max="4" width="18.28515625" style="4" customWidth="1"/>
     <col min="5" max="6" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" customWidth="1"/>
-    <col min="14" max="14" width="20" customWidth="1"/>
-    <col min="15" max="15" width="15.28515625" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
+      <c r="G1" t="s">
+        <v>24</v>
       </c>
       <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>28</v>
-      </c>
-      <c r="K1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" t="s">
-        <v>29</v>
       </c>
       <c r="M1" t="s">
         <v>30</v>
       </c>
       <c r="N1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="O1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3">
         <v>21</v>
@@ -593,38 +589,38 @@
       <c r="F2" t="s">
         <v>0</v>
       </c>
+      <c r="G2">
+        <v>0.45312000000000002</v>
+      </c>
       <c r="H2">
-        <v>0.45312000000000002</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="I2">
-        <v>0.34200000000000003</v>
+        <v>0.31</v>
       </c>
       <c r="J2">
-        <v>0.31</v>
+        <v>3.1E-2</v>
       </c>
       <c r="K2">
-        <v>3.1E-2</v>
-      </c>
-      <c r="L2">
         <f>AVERAGE(-0.08844,-0.08865)</f>
         <v>-8.8545000000000013E-2</v>
       </c>
+      <c r="L2">
+        <v>6.5199999999999998E-3</v>
+      </c>
       <c r="M2">
-        <v>6.5199999999999998E-3</v>
+        <v>0.03</v>
       </c>
       <c r="N2">
-        <v>0.03</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="O2">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="P2">
         <v>-59</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3">
         <v>22</v>
@@ -641,35 +637,35 @@
       <c r="F3" t="s">
         <v>0</v>
       </c>
+      <c r="G3">
+        <v>0.43767</v>
+      </c>
       <c r="H3">
-        <v>0.43767</v>
+        <v>0.33154</v>
       </c>
       <c r="I3">
-        <v>0.33154</v>
+        <v>0.30127999999999999</v>
       </c>
       <c r="J3">
-        <v>0.30127999999999999</v>
+        <v>3.1E-2</v>
       </c>
       <c r="K3">
-        <v>3.1E-2</v>
-      </c>
-      <c r="L3">
         <f>AVERAGE(-0.08844,-0.08211)</f>
         <v>-8.5275000000000004E-2</v>
       </c>
+      <c r="L3">
+        <v>5.7999999999999996E-3</v>
+      </c>
       <c r="M3">
-        <v>5.7999999999999996E-3</v>
+        <v>0.03</v>
       </c>
       <c r="N3">
-        <v>0.03</v>
-      </c>
-      <c r="O3">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>18</v>
@@ -686,34 +682,34 @@
       <c r="F4" t="s">
         <v>0</v>
       </c>
+      <c r="G4">
+        <v>0.41942000000000002</v>
+      </c>
       <c r="H4">
-        <v>0.41942000000000002</v>
+        <v>0.31646999999999997</v>
       </c>
       <c r="I4">
-        <v>0.31646999999999997</v>
+        <v>0.28684999999999999</v>
       </c>
       <c r="J4">
-        <v>0.28684999999999999</v>
+        <v>3.1E-2</v>
       </c>
       <c r="K4">
-        <v>3.1E-2</v>
+        <v>-8.2110000000000002E-2</v>
       </c>
       <c r="L4">
-        <v>-8.2110000000000002E-2</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="M4">
-        <v>5.7999999999999996E-3</v>
+        <v>0.03</v>
       </c>
       <c r="N4">
-        <v>0.03</v>
-      </c>
-      <c r="O4">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>21</v>
@@ -730,34 +726,34 @@
       <c r="F5" t="s">
         <v>0</v>
       </c>
+      <c r="G5">
+        <v>0.41478999999999999</v>
+      </c>
       <c r="H5">
-        <v>0.41478999999999999</v>
+        <v>0.31333</v>
       </c>
       <c r="I5">
-        <v>0.31333</v>
+        <v>0.28355000000000002</v>
       </c>
       <c r="J5">
-        <v>0.28355000000000002</v>
+        <v>3.1E-2</v>
       </c>
       <c r="K5">
-        <v>3.1E-2</v>
+        <v>-7.9909999999999995E-2</v>
       </c>
       <c r="L5">
-        <v>-7.9909999999999995E-2</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="M5">
-        <v>5.7999999999999996E-3</v>
+        <v>0.03</v>
       </c>
       <c r="N5">
-        <v>0.03</v>
-      </c>
-      <c r="O5">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <v>20</v>
@@ -774,34 +770,34 @@
       <c r="F6" t="s">
         <v>0</v>
       </c>
+      <c r="G6">
+        <v>0.40855999999999998</v>
+      </c>
       <c r="H6">
-        <v>0.40855999999999998</v>
+        <v>0.30842999999999998</v>
       </c>
       <c r="I6">
-        <v>0.30842999999999998</v>
+        <v>0.27961999999999998</v>
       </c>
       <c r="J6">
-        <v>0.27961999999999998</v>
+        <v>3.1E-2</v>
       </c>
       <c r="K6">
-        <v>3.1E-2</v>
+        <v>-7.9909999999999995E-2</v>
       </c>
       <c r="L6">
-        <v>-7.9909999999999995E-2</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="M6">
-        <v>5.7999999999999996E-3</v>
+        <v>0.03</v>
       </c>
       <c r="N6">
-        <v>0.03</v>
-      </c>
-      <c r="O6">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>19</v>
@@ -818,34 +814,34 @@
       <c r="F7" t="s">
         <v>0</v>
       </c>
+      <c r="G7">
+        <v>0.43103000000000002</v>
+      </c>
       <c r="H7">
-        <v>0.43103000000000002</v>
+        <v>0.32754</v>
       </c>
       <c r="I7">
-        <v>0.32754</v>
+        <v>0.16361000000000001</v>
       </c>
       <c r="J7">
-        <v>0.16361000000000001</v>
+        <v>3.1E-2</v>
       </c>
       <c r="K7">
-        <v>3.1E-2</v>
+        <v>-7.9909999999999995E-2</v>
       </c>
       <c r="L7">
-        <v>-7.9909999999999995E-2</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="M7">
-        <v>5.7999999999999996E-3</v>
+        <v>0.03</v>
       </c>
       <c r="N7">
-        <v>0.03</v>
-      </c>
-      <c r="O7">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
         <v>20</v>
@@ -862,37 +858,37 @@
       <c r="F8" t="s">
         <v>0</v>
       </c>
+      <c r="G8">
+        <v>0.49356</v>
+      </c>
       <c r="H8">
-        <v>0.49356</v>
+        <v>0.33291999999999999</v>
       </c>
       <c r="I8">
-        <v>0.33291999999999999</v>
+        <v>0.16078000000000001</v>
       </c>
       <c r="J8">
-        <v>0.16078000000000001</v>
+        <v>3.1E-2</v>
       </c>
       <c r="K8">
-        <v>3.1E-2</v>
+        <v>-7.9909999999999995E-2</v>
       </c>
       <c r="L8">
-        <v>-7.9909999999999995E-2</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="M8">
-        <v>5.7999999999999996E-3</v>
+        <v>0.03</v>
       </c>
       <c r="N8">
-        <v>0.03</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="O8">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="P8">
         <v>-29</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>20</v>
@@ -909,34 +905,34 @@
       <c r="F9" t="s">
         <v>0</v>
       </c>
+      <c r="G9">
+        <v>0.60599999999999998</v>
+      </c>
       <c r="H9">
-        <v>0.60599999999999998</v>
+        <v>0.34449000000000002</v>
       </c>
       <c r="I9">
-        <v>0.34449000000000002</v>
+        <v>0.15564</v>
       </c>
       <c r="J9">
-        <v>0.15564</v>
+        <v>3.1E-2</v>
       </c>
       <c r="K9">
-        <v>3.1E-2</v>
+        <v>-7.9909999999999995E-2</v>
       </c>
       <c r="L9">
-        <v>-7.9909999999999995E-2</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="M9">
-        <v>5.7999999999999996E-3</v>
+        <v>0.03</v>
       </c>
       <c r="N9">
-        <v>0.03</v>
-      </c>
-      <c r="O9">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>19</v>
@@ -953,34 +949,34 @@
       <c r="F10" t="s">
         <v>0</v>
       </c>
+      <c r="G10">
+        <v>0.60355999999999999</v>
+      </c>
       <c r="H10">
-        <v>0.60355999999999999</v>
+        <v>0.34188000000000002</v>
       </c>
       <c r="I10">
-        <v>0.34188000000000002</v>
+        <v>0.15367</v>
       </c>
       <c r="J10">
-        <v>0.15367</v>
+        <v>3.1E-2</v>
       </c>
       <c r="K10">
-        <v>3.1E-2</v>
+        <v>-7.9909999999999995E-2</v>
       </c>
       <c r="L10">
-        <v>-7.9909999999999995E-2</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="M10">
-        <v>5.7999999999999996E-3</v>
+        <v>0.03</v>
       </c>
       <c r="N10">
-        <v>0.03</v>
-      </c>
-      <c r="O10">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>21</v>
@@ -997,32 +993,32 @@
       <c r="F11" t="s">
         <v>0</v>
       </c>
+      <c r="G11">
+        <v>0.60365000000000002</v>
+      </c>
       <c r="H11">
-        <v>0.60365000000000002</v>
+        <v>0.34184999999999999</v>
       </c>
       <c r="I11">
-        <v>0.34184999999999999</v>
+        <v>0.15368000000000001</v>
       </c>
       <c r="J11">
-        <v>0.15368000000000001</v>
+        <v>3.1E-2</v>
       </c>
       <c r="K11">
-        <v>3.1E-2</v>
+        <v>-7.9909999999999995E-2</v>
       </c>
       <c r="L11">
-        <v>-7.9909999999999995E-2</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="M11">
-        <v>5.7999999999999996E-3</v>
+        <v>0.03</v>
       </c>
       <c r="N11">
-        <v>0.03</v>
-      </c>
-      <c r="O11">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1041,34 +1037,34 @@
       <c r="F12" t="s">
         <v>0</v>
       </c>
+      <c r="G12">
+        <v>0.52863000000000004</v>
+      </c>
       <c r="H12">
-        <v>0.52863000000000004</v>
+        <v>0.32258999999999999</v>
       </c>
       <c r="I12">
-        <v>0.32258999999999999</v>
+        <v>0.15315000000000001</v>
       </c>
       <c r="J12">
-        <v>0.15315000000000001</v>
+        <v>3.1E-2</v>
       </c>
       <c r="K12">
-        <v>3.1E-2</v>
+        <v>-7.2989999999999999E-2</v>
       </c>
       <c r="L12">
-        <v>-7.2989999999999999E-2</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="M12">
-        <v>5.7999999999999996E-3</v>
+        <v>0.03</v>
       </c>
       <c r="N12">
-        <v>0.03</v>
-      </c>
-      <c r="O12">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="2">
         <v>20</v>
@@ -1085,19 +1081,19 @@
       <c r="F13" t="s">
         <v>0</v>
       </c>
+      <c r="G13">
+        <v>0.39071</v>
+      </c>
       <c r="H13">
-        <v>0.39071</v>
+        <v>0.29363</v>
       </c>
       <c r="I13">
-        <v>0.29363</v>
-      </c>
-      <c r="J13">
         <v>0.15232999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="2">
         <v>21</v>
@@ -1115,9 +1111,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="2">
         <v>22</v>
@@ -1135,9 +1131,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2">
         <v>23</v>
@@ -1157,7 +1153,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="2">
         <v>23</v>
@@ -1187,7 +1183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6806A540-0326-4DB6-B9B8-16C9F67C5C5B}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1200,35 +1196,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1240,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD82D3A-F989-4706-BFEC-23F69017CEED}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,27 +1250,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -1294,7 +1290,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -1314,7 +1310,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>28</v>
@@ -1334,7 +1330,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -1354,7 +1350,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -1374,7 +1370,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>30</v>
@@ -1394,7 +1390,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>11</v>
@@ -1414,7 +1410,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>25</v>
@@ -1434,7 +1430,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -1454,7 +1450,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -1474,7 +1470,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>28</v>
@@ -1494,7 +1490,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -1514,7 +1510,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>10</v>
@@ -1534,7 +1530,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -1554,7 +1550,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16">
         <v>26</v>
@@ -1574,7 +1570,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17">
         <v>10</v>
@@ -1594,7 +1590,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -1614,7 +1610,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19">
         <v>27</v>
@@ -1634,7 +1630,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20">
         <v>13</v>
@@ -1654,7 +1650,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -1674,7 +1670,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22">
         <v>29</v>
@@ -1694,7 +1690,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23">
         <v>16</v>
@@ -1714,7 +1710,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24">
         <v>9</v>
@@ -1734,7 +1730,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1754,7 +1750,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26">
         <v>13</v>
@@ -1774,7 +1770,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27">
         <v>6</v>
@@ -1794,7 +1790,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28">
         <v>30</v>
@@ -1814,27 +1810,27 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C29">
         <v>2021</v>
       </c>
       <c r="D29" s="4">
-        <v>44201</v>
+        <v>44208</v>
       </c>
       <c r="E29">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F29">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -1846,10 +1842,10 @@
         <v>44201</v>
       </c>
       <c r="E30">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F30">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>